<commit_message>
sprint 3 updated and sprint 4 added
</commit_message>
<xml_diff>
--- a/S24 Product Backlog - updated 08112024 - TIIMI2.xlsx
+++ b/S24 Product Backlog - updated 08112024 - TIIMI2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9d8cbaf794e8c62c/Desktop/Syksy 2024 kevät 2025/OhjelmistoProjekti1/s24Tiimi2Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BF564772-1134-4C42-9029-AD4C626E3172}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="56" documentId="8_{BF564772-1134-4C42-9029-AD4C626E3172}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B23B7022-417B-45E6-970C-FF42F186A9D9}"/>
   <bookViews>
-    <workbookView xWindow="16836" yWindow="1644" windowWidth="19176" windowHeight="12120" xr2:uid="{C479CED9-8A31-459B-9A34-852820542566}"/>
+    <workbookView xWindow="28695" yWindow="180" windowWidth="21600" windowHeight="15660" xr2:uid="{C479CED9-8A31-459B-9A34-852820542566}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -217,7 +217,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="243">
   <si>
     <t>Theme</t>
   </si>
@@ -994,7 +994,34 @@
     <t>on going</t>
   </si>
   <si>
-    <t xml:space="preserve">on going </t>
+    <t>..spring boot sovelluksen käyttöliittymä on "hyvän näköinen" ja helppokäyttöinen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Käyttäjäystävällisen ja laadukkaan näköinen sovellus luo luotettavuutta koko yritystä kohden. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tiimi päättää itse, minkälainen tulee olemaan sovelluksen ulkoasu. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tiimin jäsenet ovat tyytyväisiä käyttöliittymän ulkoasuun. </t>
+  </si>
+  <si>
+    <t>e) Sovellus / Front end</t>
+  </si>
+  <si>
+    <t>loppukäyttäjän sovellus on "hyvän näköinen" ja helppokäyttöinen</t>
+  </si>
+  <si>
+    <t>kaupan asiakas voi rekisteröityä kaupan asiakkaaksi. Minimitiedot ovat etu-, sukunimi ja email osoite</t>
+  </si>
+  <si>
+    <t>ks muut tiedot vaatimuksesta 46</t>
+  </si>
+  <si>
+    <t>Sprint 4</t>
+  </si>
+  <si>
+    <t>Sprint  4</t>
   </si>
 </sst>
 </file>
@@ -1447,24 +1474,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4A41D4B-E510-47CE-BAC3-3E487078559C}">
-  <dimension ref="A1:J59"/>
+  <dimension ref="A1:J60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J39" sqref="J39"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I58" sqref="I58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="8.21875" style="8" customWidth="1"/>
-    <col min="2" max="2" width="19.77734375" customWidth="1"/>
-    <col min="3" max="3" width="13.21875" customWidth="1"/>
-    <col min="4" max="4" width="24.44140625" customWidth="1"/>
-    <col min="5" max="5" width="32.21875" customWidth="1"/>
-    <col min="6" max="6" width="34.77734375" customWidth="1"/>
-    <col min="7" max="7" width="28.77734375" customWidth="1"/>
-    <col min="8" max="8" width="9.21875" style="4"/>
-    <col min="10" max="10" width="28.77734375" customWidth="1"/>
+    <col min="1" max="1" width="8.1796875" style="8" customWidth="1"/>
+    <col min="2" max="2" width="19.81640625" customWidth="1"/>
+    <col min="3" max="3" width="13.1796875" customWidth="1"/>
+    <col min="4" max="4" width="24.453125" customWidth="1"/>
+    <col min="5" max="5" width="32.1796875" customWidth="1"/>
+    <col min="6" max="6" width="34.81640625" customWidth="1"/>
+    <col min="7" max="7" width="28.81640625" customWidth="1"/>
+    <col min="8" max="8" width="9.1796875" style="4"/>
+    <col min="10" max="10" width="28.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="90">
@@ -1531,7 +1558,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="68.55" customHeight="1">
+    <row r="3" spans="1:10" ht="68.5" customHeight="1">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1563,7 +1590,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="73.95" customHeight="1">
+    <row r="4" spans="1:10" ht="74" customHeight="1">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1595,7 +1622,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="91.95" customHeight="1">
+    <row r="5" spans="1:10" ht="92" customHeight="1">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1659,7 +1686,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="70.95" customHeight="1">
+    <row r="7" spans="1:10" ht="71" customHeight="1">
       <c r="A7" s="7">
         <v>6</v>
       </c>
@@ -1723,7 +1750,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="62.55" customHeight="1">
+    <row r="9" spans="1:10" ht="62.5" customHeight="1">
       <c r="A9" s="7">
         <v>8</v>
       </c>
@@ -1755,7 +1782,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="84.6" customHeight="1">
+    <row r="10" spans="1:10" ht="84.65" customHeight="1">
       <c r="A10" s="7">
         <v>9</v>
       </c>
@@ -1787,7 +1814,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="62.55" customHeight="1">
+    <row r="11" spans="1:10" ht="62.5" customHeight="1">
       <c r="A11" s="7">
         <v>10</v>
       </c>
@@ -1851,7 +1878,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="63.6" customHeight="1">
+    <row r="13" spans="1:10" ht="63.65" customHeight="1">
       <c r="A13" s="7">
         <v>12</v>
       </c>
@@ -2011,7 +2038,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="78.599999999999994" customHeight="1">
+    <row r="18" spans="1:10" ht="78.650000000000006" customHeight="1">
       <c r="A18" s="7">
         <v>17</v>
       </c>
@@ -2068,8 +2095,12 @@
       <c r="H19" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
+      <c r="I19" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>241</v>
+      </c>
     </row>
     <row r="20" spans="1:10" ht="84.75" customHeight="1">
       <c r="A20" s="7">
@@ -2103,7 +2134,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="110.4">
+    <row r="21" spans="1:10" ht="98">
       <c r="A21" s="7">
         <v>20</v>
       </c>
@@ -2195,7 +2226,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="69">
+    <row r="24" spans="1:10" ht="70">
       <c r="A24" s="7">
         <v>23</v>
       </c>
@@ -2223,7 +2254,7 @@
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
     </row>
-    <row r="25" spans="1:10" ht="69">
+    <row r="25" spans="1:10" ht="70">
       <c r="A25" s="7">
         <v>24</v>
       </c>
@@ -2251,7 +2282,7 @@
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
     </row>
-    <row r="26" spans="1:10" ht="105.6" customHeight="1">
+    <row r="26" spans="1:10" ht="105.65" customHeight="1">
       <c r="A26" s="7">
         <v>25</v>
       </c>
@@ -2283,7 +2314,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="73.95" customHeight="1">
+    <row r="27" spans="1:10" ht="74" customHeight="1">
       <c r="A27" s="7">
         <v>26</v>
       </c>
@@ -2372,8 +2403,12 @@
       <c r="H29" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="I29" s="2"/>
-      <c r="J29" s="2"/>
+      <c r="I29" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>241</v>
+      </c>
     </row>
     <row r="30" spans="1:10" ht="76.5" customHeight="1">
       <c r="A30" s="7">
@@ -2400,10 +2435,14 @@
       <c r="H30" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="I30" s="2"/>
-      <c r="J30" s="2"/>
-    </row>
-    <row r="31" spans="1:10" ht="61.95" customHeight="1">
+      <c r="I30" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="62" customHeight="1">
       <c r="A31" s="7">
         <v>30</v>
       </c>
@@ -2428,10 +2467,14 @@
       <c r="H31" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="I31" s="2"/>
-      <c r="J31" s="2"/>
-    </row>
-    <row r="32" spans="1:10" ht="71.099999999999994" customHeight="1">
+      <c r="I31" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="71.150000000000006" customHeight="1">
       <c r="A32" s="7">
         <v>31</v>
       </c>
@@ -2456,14 +2499,14 @@
       <c r="H32" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="I32" s="2" t="s">
-        <v>232</v>
+      <c r="I32" s="10" t="s">
+        <v>215</v>
       </c>
       <c r="J32" s="2" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="74.099999999999994" customHeight="1">
+    <row r="33" spans="1:10" ht="74.150000000000006" customHeight="1">
       <c r="A33" s="7">
         <v>32</v>
       </c>
@@ -2488,8 +2531,8 @@
       <c r="H33" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I33" s="2" t="s">
-        <v>232</v>
+      <c r="I33" s="10" t="s">
+        <v>215</v>
       </c>
       <c r="J33" s="2" t="s">
         <v>231</v>
@@ -2552,14 +2595,14 @@
       <c r="H35" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="I35" s="2" t="s">
-        <v>232</v>
+      <c r="I35" s="10" t="s">
+        <v>215</v>
       </c>
       <c r="J35" s="2" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="137.55000000000001" customHeight="1">
+    <row r="36" spans="1:10" ht="137.5" customHeight="1">
       <c r="A36" s="7">
         <v>35</v>
       </c>
@@ -2591,7 +2634,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="95.55" customHeight="1">
+    <row r="37" spans="1:10" ht="95.5" customHeight="1">
       <c r="A37" s="7">
         <v>36</v>
       </c>
@@ -2623,7 +2666,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="73.05" customHeight="1">
+    <row r="38" spans="1:10" ht="73" customHeight="1">
       <c r="A38" s="7">
         <v>37</v>
       </c>
@@ -2655,7 +2698,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="86.55" customHeight="1">
+    <row r="39" spans="1:10" ht="86.5" customHeight="1">
       <c r="A39" s="7">
         <v>38</v>
       </c>
@@ -2715,7 +2758,7 @@
       <c r="I40" s="2"/>
       <c r="J40" s="2"/>
     </row>
-    <row r="41" spans="1:10" ht="109.2" customHeight="1">
+    <row r="41" spans="1:10" ht="109.25" customHeight="1">
       <c r="A41" s="7">
         <v>40</v>
       </c>
@@ -2740,8 +2783,12 @@
       <c r="H41" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="I41" s="2"/>
-      <c r="J41" s="2"/>
+      <c r="I41" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="J41" s="2" t="s">
+        <v>241</v>
+      </c>
     </row>
     <row r="42" spans="1:10" ht="84" customHeight="1">
       <c r="A42" s="7">
@@ -2771,7 +2818,7 @@
       <c r="I42" s="2"/>
       <c r="J42" s="2"/>
     </row>
-    <row r="43" spans="1:10" ht="55.2">
+    <row r="43" spans="1:10" ht="56">
       <c r="A43" s="7">
         <v>42</v>
       </c>
@@ -2796,10 +2843,14 @@
       <c r="H43" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="I43" s="2"/>
-      <c r="J43" s="2"/>
-    </row>
-    <row r="44" spans="1:10" ht="71.55" customHeight="1">
+      <c r="I43" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="J43" s="2" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" ht="71.5" customHeight="1">
       <c r="A44" s="7">
         <v>43</v>
       </c>
@@ -2824,10 +2875,14 @@
       <c r="H44" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="I44" s="2"/>
-      <c r="J44" s="2"/>
-    </row>
-    <row r="45" spans="1:10" ht="55.2">
+      <c r="I44" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="J44" s="2" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" ht="56">
       <c r="A45" s="7">
         <v>44</v>
       </c>
@@ -2852,10 +2907,14 @@
       <c r="H45" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="I45" s="2"/>
-      <c r="J45" s="2"/>
-    </row>
-    <row r="46" spans="1:10" ht="69">
+      <c r="I45" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="J45" s="2" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" ht="56">
       <c r="A46" s="7">
         <v>45</v>
       </c>
@@ -2880,10 +2939,14 @@
       <c r="H46" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="I46" s="2"/>
-      <c r="J46" s="2"/>
-    </row>
-    <row r="47" spans="1:10" ht="69">
+      <c r="I46" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="J46" s="2" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" ht="70">
       <c r="A47" s="7">
         <v>46</v>
       </c>
@@ -2908,10 +2971,14 @@
       <c r="H47" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="I47" s="2"/>
-      <c r="J47" s="2"/>
-    </row>
-    <row r="48" spans="1:10" ht="95.1" customHeight="1">
+      <c r="I47" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="J47" s="2" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" ht="95.15" customHeight="1">
       <c r="A48" s="7">
         <v>47</v>
       </c>
@@ -2936,14 +3003,14 @@
       <c r="H48" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I48" s="2" t="s">
-        <v>232</v>
+      <c r="I48" s="10" t="s">
+        <v>215</v>
       </c>
       <c r="J48" s="2" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="49" spans="1:10" ht="166.95" customHeight="1">
+    <row r="49" spans="1:10" ht="167" customHeight="1">
       <c r="A49" s="7">
         <v>48</v>
       </c>
@@ -2968,10 +3035,14 @@
       <c r="H49" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="I49" s="2"/>
-      <c r="J49" s="2"/>
-    </row>
-    <row r="50" spans="1:10" ht="59.55" customHeight="1">
+      <c r="I49" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="J49" s="2" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" ht="59.5" customHeight="1">
       <c r="A50" s="7">
         <v>49</v>
       </c>
@@ -2996,10 +3067,14 @@
       <c r="H50" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="I50" s="2"/>
-      <c r="J50" s="2"/>
-    </row>
-    <row r="51" spans="1:10" ht="96.6">
+      <c r="I50" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="J50" s="2" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" ht="98">
       <c r="A51" s="7">
         <v>50</v>
       </c>
@@ -3024,8 +3099,12 @@
       <c r="H51" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I51" s="2"/>
-      <c r="J51" s="2"/>
+      <c r="I51" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="J51" s="2" t="s">
+        <v>230</v>
+      </c>
     </row>
     <row r="52" spans="1:10" ht="118.5" customHeight="1">
       <c r="A52" s="7">
@@ -3052,8 +3131,8 @@
       <c r="H52" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I52" s="2" t="s">
-        <v>233</v>
+      <c r="I52" s="10" t="s">
+        <v>215</v>
       </c>
       <c r="J52" s="2" t="s">
         <v>231</v>
@@ -3084,14 +3163,14 @@
       <c r="H53" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I53" s="2" t="s">
-        <v>232</v>
+      <c r="I53" s="10" t="s">
+        <v>215</v>
       </c>
       <c r="J53" s="2" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="54" spans="1:10" ht="55.2">
+    <row r="54" spans="1:10" ht="56">
       <c r="A54" s="7">
         <v>53</v>
       </c>
@@ -3116,8 +3195,8 @@
       <c r="H54" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I54" s="2" t="s">
-        <v>232</v>
+      <c r="I54" s="10" t="s">
+        <v>215</v>
       </c>
       <c r="J54" s="2" t="s">
         <v>231</v>
@@ -3187,7 +3266,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="57" spans="1:10" ht="69">
+    <row r="57" spans="1:10" ht="70">
       <c r="A57" s="7">
         <v>56</v>
       </c>
@@ -3219,33 +3298,97 @@
         <v>230</v>
       </c>
     </row>
-    <row r="58" spans="1:10">
+    <row r="58" spans="1:10" ht="70">
       <c r="A58" s="7">
         <v>57</v>
       </c>
-      <c r="B58" s="3"/>
-      <c r="C58" s="3"/>
-      <c r="D58" s="3"/>
-      <c r="E58" s="3"/>
-      <c r="F58" s="3"/>
-      <c r="G58" s="3"/>
-      <c r="H58" s="2"/>
-      <c r="I58" s="2"/>
-      <c r="J58" s="3"/>
-    </row>
-    <row r="59" spans="1:10">
+      <c r="B58" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="F58" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="G58" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="H58" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I58" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="J58" s="2" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" ht="56">
       <c r="A59" s="7">
         <v>58</v>
       </c>
-      <c r="B59" s="3"/>
-      <c r="C59" s="3"/>
-      <c r="D59" s="3"/>
-      <c r="E59" s="3"/>
-      <c r="F59" s="3"/>
-      <c r="G59" s="3"/>
-      <c r="H59" s="2"/>
-      <c r="I59" s="2"/>
-      <c r="J59" s="3"/>
+      <c r="B59" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="F59" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="G59" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="H59" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I59" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="J59" s="2" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" ht="84">
+      <c r="A60" s="7">
+        <v>59</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="F60" s="3"/>
+      <c r="G60" s="3"/>
+      <c r="H60" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="I60" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="J60" s="2" t="s">
+        <v>241</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:J59" xr:uid="{E4A41D4B-E510-47CE-BAC3-3E487078559C}"/>
@@ -3262,6 +3405,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="5041c815-b662-4e97-91f9-dfea5c801e6c" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010000F31C13F2B02C42804791B7D176580F" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b758590bad793664214290192af8eea1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="5041c815-b662-4e97-91f9-dfea5c801e6c" xmlns:ns4="6f4f8b50-ea0e-40fb-af4c-f58df4ea5ac5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="37d8109bda380f817570ff6b57111f4d" ns3:_="" ns4:_="">
     <xsd:import namespace="5041c815-b662-4e97-91f9-dfea5c801e6c"/>
@@ -3514,24 +3674,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0269E476-3EF6-4749-ADF3-0D5C450A2E68}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="6f4f8b50-ea0e-40fb-af4c-f58df4ea5ac5"/>
+    <ds:schemaRef ds:uri="5041c815-b662-4e97-91f9-dfea5c801e6c"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="5041c815-b662-4e97-91f9-dfea5c801e6c" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FEE8F6A6-0841-43B9-BEE5-4DB5A1480306}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F9D0DAEF-B02C-4FAE-8C8C-9001DE1D1DA5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3548,29 +3716,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FEE8F6A6-0841-43B9-BEE5-4DB5A1480306}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0269E476-3EF6-4749-ADF3-0D5C450A2E68}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="6f4f8b50-ea0e-40fb-af4c-f58df4ea5ac5"/>
-    <ds:schemaRef ds:uri="5041c815-b662-4e97-91f9-dfea5c801e6c"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>